<commit_message>
There are 12 antennas on the rooftop, calculate the received power on each point on the rooftop and draw the distribution.
</commit_message>
<xml_diff>
--- a/antenna12.xlsx
+++ b/antenna12.xlsx
@@ -20,7 +20,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,6 +33,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -56,8 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -345,208 +353,211 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>110</v>
-      </c>
-      <c r="B1">
-        <v>60</v>
-      </c>
-      <c r="C1">
+      <c r="A1" s="1">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1">
         <v>5</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
+        <v>-80</v>
+      </c>
+      <c r="E1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-210</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-300</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-150</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-265</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-120</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-240</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
         <v>-70</v>
       </c>
-      <c r="E1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>110</v>
-      </c>
-      <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
         <v>-210</v>
       </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>110</v>
-      </c>
-      <c r="B3">
-        <v>60</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="E11" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
         <v>-300</v>
       </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>210</v>
-      </c>
-      <c r="B4">
-        <v>140</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>-5</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>210</v>
-      </c>
-      <c r="B5">
-        <v>140</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>-150</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>210</v>
-      </c>
-      <c r="B6">
-        <v>140</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>-265</v>
-      </c>
-      <c r="E6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>320</v>
-      </c>
-      <c r="B7">
-        <v>70</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>320</v>
-      </c>
-      <c r="B8">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>-120</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>320</v>
-      </c>
-      <c r="B9">
-        <v>70</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>-240</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>430</v>
-      </c>
-      <c r="B10">
-        <v>130</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>-70</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>430</v>
-      </c>
-      <c r="B11">
-        <v>130</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11">
-        <v>-210</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>430</v>
-      </c>
-      <c r="B12">
-        <v>130</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>-300</v>
-      </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>8</v>
       </c>
     </row>

</xml_diff>